<commit_message>
Added cmip6 mapings for cmip5 atmosphere key properties.  Corrected atmos_solar.py specializations for orbital parameters.
</commit_message>
<xml_diff>
--- a/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
-  <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-atmos/mappings/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="28480" yWindow="740" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="139">
   <si>
     <t>Atmosphere &gt; Convection Cloud Turbulence</t>
   </si>
@@ -417,13 +412,40 @@
   </si>
   <si>
     <t>CMIP6 Specialization ID</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar/insolation_ozone.solar_ozone_impact</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.orbital_parameters.computation_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.orbital_parameters.fixed_reference_date</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.orbital_parameters.type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.solar_constant.fixed_value</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.orbital_parameters.transient_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.solar_constant.transient_characteristics</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.solar_constant.type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.volcanos.volcanoes_treatment.volcanoes_implementation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -444,6 +466,23 @@
     <font>
       <sz val="18"/>
       <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
@@ -467,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -535,13 +574,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA5A5A5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -563,8 +647,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1754,9 +1851,11 @@
   </sheetPr>
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="51.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1764,7 +1863,7 @@
     <col min="4" max="254" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="27" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>127</v>
       </c>
@@ -1775,7 +1874,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>126</v>
       </c>
@@ -1786,7 +1885,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>126</v>
       </c>
@@ -1797,7 +1896,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>126</v>
       </c>
@@ -1808,7 +1907,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>126</v>
       </c>
@@ -1819,34 +1918,40 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C6" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C7" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C8" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>126</v>
       </c>
@@ -1855,7 +1960,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>126</v>
       </c>
@@ -1864,34 +1969,40 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C11" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C12" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C13" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>126</v>
       </c>
@@ -1900,52 +2011,62 @@
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C15" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C16" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C17" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C18" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C19" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="20" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>126</v>
       </c>
@@ -1954,7 +2075,7 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="20" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>126</v>
       </c>
@@ -1963,12 +2084,12 @@
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="20" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="20.25" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -1977,7 +2098,7 @@
       </c>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="20.25" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -1986,7 +2107,7 @@
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="20.25" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +2116,7 @@
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="20.25" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -2004,7 +2125,7 @@
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="20.25" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -2013,7 +2134,7 @@
       </c>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="20.25" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2143,7 @@
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="20.25" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -2031,7 +2152,7 @@
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="20.25" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -2040,7 +2161,7 @@
       </c>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="20.25" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2049,7 +2170,7 @@
       </c>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="20.25" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2058,7 +2179,7 @@
       </c>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="20.25" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2067,7 +2188,7 @@
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="20.25" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -2076,7 +2197,7 @@
       </c>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="20.25" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -2085,7 +2206,7 @@
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="20.25" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -2094,7 +2215,7 @@
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="20.25" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -2103,7 +2224,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="20.25" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2233,7 @@
       </c>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="20.25" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
@@ -2121,7 +2242,7 @@
       </c>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="20.25" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
@@ -2130,12 +2251,12 @@
       </c>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="20.25" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="20.25" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
@@ -2144,7 +2265,7 @@
       </c>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="20.25" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>1</v>
       </c>
@@ -2153,7 +2274,7 @@
       </c>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" ht="20.25" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>1</v>
       </c>
@@ -2164,7 +2285,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" ht="20.25" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
@@ -2173,7 +2294,7 @@
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" ht="20.25" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>1</v>
       </c>
@@ -2182,7 +2303,7 @@
       </c>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" ht="20.25" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>1</v>
       </c>
@@ -2193,7 +2314,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="20.25" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
@@ -2204,7 +2325,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="20.25" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>1</v>
       </c>
@@ -2215,7 +2336,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="20.25" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
@@ -2226,12 +2347,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="20.25" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="20.25" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
@@ -2240,7 +2361,7 @@
       </c>
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" ht="20.25" customHeight="1">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
@@ -2249,7 +2370,7 @@
       </c>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" ht="20.25" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>2</v>
       </c>
@@ -2258,7 +2379,7 @@
       </c>
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3" ht="20.25" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
@@ -2267,7 +2388,7 @@
       </c>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" ht="20.25" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2278,7 +2399,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" ht="20.25" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
@@ -2289,7 +2410,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" ht="20.25" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
@@ -2298,7 +2419,7 @@
       </c>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" ht="20.25" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
@@ -2307,7 +2428,7 @@
       </c>
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" ht="20.25" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
@@ -2316,7 +2437,7 @@
       </c>
       <c r="C60" s="4"/>
     </row>
-    <row r="61" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:3" ht="20.25" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
@@ -2325,7 +2446,7 @@
       </c>
       <c r="C61" s="4"/>
     </row>
-    <row r="62" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3" ht="20.25" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -2334,7 +2455,7 @@
       </c>
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:3" ht="20.25" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -2343,12 +2464,12 @@
       </c>
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3" ht="20.25" customHeight="1">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" ht="20.25" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>3</v>
       </c>
@@ -2357,7 +2478,7 @@
       </c>
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:3" ht="20.25" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>3</v>
       </c>
@@ -2366,7 +2487,7 @@
       </c>
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:3" ht="20.25" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>3</v>
       </c>
@@ -2375,7 +2496,7 @@
       </c>
       <c r="C67" s="4"/>
     </row>
-    <row r="68" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:3" ht="20.25" customHeight="1">
       <c r="A68" s="2" t="s">
         <v>3</v>
       </c>
@@ -2384,7 +2505,7 @@
       </c>
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:3" ht="20.25" customHeight="1">
       <c r="A69" s="2" t="s">
         <v>3</v>
       </c>
@@ -2393,7 +2514,7 @@
       </c>
       <c r="C69" s="4"/>
     </row>
-    <row r="70" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:3" ht="20.25" customHeight="1">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -2402,7 +2523,7 @@
       </c>
       <c r="C70" s="4"/>
     </row>
-    <row r="71" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:3" ht="20.25" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -2411,7 +2532,7 @@
       </c>
       <c r="C71" s="4"/>
     </row>
-    <row r="72" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:3" ht="20.25" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>3</v>
       </c>
@@ -2420,7 +2541,7 @@
       </c>
       <c r="C72" s="4"/>
     </row>
-    <row r="73" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:3" ht="20.25" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>3</v>
       </c>
@@ -2429,7 +2550,7 @@
       </c>
       <c r="C73" s="4"/>
     </row>
-    <row r="74" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:3" ht="20.25" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>3</v>
       </c>
@@ -2438,7 +2559,7 @@
       </c>
       <c r="C74" s="4"/>
     </row>
-    <row r="75" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:3" ht="20.25" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>3</v>
       </c>
@@ -2447,7 +2568,7 @@
       </c>
       <c r="C75" s="4"/>
     </row>
-    <row r="76" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:3" ht="20.25" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -2456,7 +2577,7 @@
       </c>
       <c r="C76" s="4"/>
     </row>
-    <row r="77" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:3" ht="20.25" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>3</v>
       </c>
@@ -2465,12 +2586,12 @@
       </c>
       <c r="C77" s="4"/>
     </row>
-    <row r="78" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:3" ht="20.25" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:3" ht="20.25" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>4</v>
       </c>
@@ -2479,7 +2600,7 @@
       </c>
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:3" ht="20.25" customHeight="1">
       <c r="A80" s="2" t="s">
         <v>4</v>
       </c>
@@ -2488,7 +2609,7 @@
       </c>
       <c r="C80" s="4"/>
     </row>
-    <row r="81" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:3" ht="20.25" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>4</v>
       </c>
@@ -2497,7 +2618,7 @@
       </c>
       <c r="C81" s="4"/>
     </row>
-    <row r="82" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:3" ht="20.25" customHeight="1">
       <c r="A82" s="2" t="s">
         <v>4</v>
       </c>
@@ -2506,7 +2627,7 @@
       </c>
       <c r="C82" s="4"/>
     </row>
-    <row r="83" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:3" ht="20.25" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>4</v>
       </c>
@@ -2515,7 +2636,7 @@
       </c>
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:3" ht="20.25" customHeight="1">
       <c r="A84" s="2" t="s">
         <v>4</v>
       </c>
@@ -2524,7 +2645,7 @@
       </c>
       <c r="C84" s="4"/>
     </row>
-    <row r="85" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:3" ht="20.25" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>4</v>
       </c>
@@ -2533,7 +2654,7 @@
       </c>
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:3" ht="20.25" customHeight="1">
       <c r="A86" s="2" t="s">
         <v>4</v>
       </c>
@@ -2542,7 +2663,7 @@
       </c>
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:3" ht="20.25" customHeight="1">
       <c r="A87" s="2" t="s">
         <v>4</v>
       </c>
@@ -2551,7 +2672,7 @@
       </c>
       <c r="C87" s="4"/>
     </row>
-    <row r="88" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:3" ht="20.25" customHeight="1">
       <c r="A88" s="2" t="s">
         <v>4</v>
       </c>
@@ -2560,12 +2681,12 @@
       </c>
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:3" ht="20.25" customHeight="1">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:3" ht="20.25" customHeight="1">
       <c r="A90" s="2" t="s">
         <v>5</v>
       </c>
@@ -2574,7 +2695,7 @@
       </c>
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:3" ht="20.25" customHeight="1">
       <c r="A91" s="2" t="s">
         <v>5</v>
       </c>
@@ -2583,7 +2704,7 @@
       </c>
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:3" ht="20.25" customHeight="1">
       <c r="A92" s="2" t="s">
         <v>5</v>
       </c>
@@ -2592,7 +2713,7 @@
       </c>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:3" ht="20.25" customHeight="1">
       <c r="A93" s="2" t="s">
         <v>5</v>
       </c>
@@ -2601,7 +2722,7 @@
       </c>
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:3" ht="20.25" customHeight="1">
       <c r="A94" s="2" t="s">
         <v>5</v>
       </c>
@@ -2610,7 +2731,7 @@
       </c>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:3" ht="20.25" customHeight="1">
       <c r="A95" s="2" t="s">
         <v>5</v>
       </c>
@@ -2619,7 +2740,7 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:3" ht="20.25" customHeight="1">
       <c r="A96" s="2" t="s">
         <v>5</v>
       </c>
@@ -2628,7 +2749,7 @@
       </c>
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:3" ht="20.25" customHeight="1">
       <c r="A97" s="2" t="s">
         <v>5</v>
       </c>
@@ -2637,7 +2758,7 @@
       </c>
       <c r="C97" s="4"/>
     </row>
-    <row r="98" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:3" ht="20.25" customHeight="1">
       <c r="A98" s="2" t="s">
         <v>5</v>
       </c>
@@ -2646,7 +2767,7 @@
       </c>
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:3" ht="20.25" customHeight="1">
       <c r="A99" s="2" t="s">
         <v>5</v>
       </c>
@@ -2655,7 +2776,7 @@
       </c>
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:3" ht="20.25" customHeight="1">
       <c r="A100" s="2" t="s">
         <v>5</v>
       </c>
@@ -2664,7 +2785,7 @@
       </c>
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:3" ht="20.25" customHeight="1">
       <c r="A101" s="2" t="s">
         <v>5</v>
       </c>
@@ -2673,7 +2794,7 @@
       </c>
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:3" ht="20.25" customHeight="1">
       <c r="A102" s="2" t="s">
         <v>5</v>
       </c>
@@ -2682,7 +2803,7 @@
       </c>
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:3" ht="20.25" customHeight="1">
       <c r="A103" s="2" t="s">
         <v>5</v>
       </c>
@@ -2691,12 +2812,12 @@
       </c>
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:3" ht="20.25" customHeight="1">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:3" ht="20.25" customHeight="1">
       <c r="A105" s="2" t="s">
         <v>6</v>
       </c>
@@ -2705,7 +2826,7 @@
       </c>
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:3" ht="20.25" customHeight="1">
       <c r="A106" s="2" t="s">
         <v>6</v>
       </c>
@@ -2714,7 +2835,7 @@
       </c>
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:3" ht="20.25" customHeight="1">
       <c r="A107" s="2" t="s">
         <v>6</v>
       </c>
@@ -2723,7 +2844,7 @@
       </c>
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:3" ht="20.25" customHeight="1">
       <c r="A108" s="2" t="s">
         <v>6</v>
       </c>
@@ -2732,7 +2853,7 @@
       </c>
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:3" ht="20.25" customHeight="1">
       <c r="A109" s="2" t="s">
         <v>6</v>
       </c>
@@ -2741,7 +2862,7 @@
       </c>
       <c r="C109" s="4"/>
     </row>
-    <row r="110" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:3" ht="20.25" customHeight="1">
       <c r="A110" s="2" t="s">
         <v>6</v>
       </c>
@@ -2750,7 +2871,7 @@
       </c>
       <c r="C110" s="4"/>
     </row>
-    <row r="111" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:3" ht="20.25" customHeight="1">
       <c r="A111" s="2" t="s">
         <v>6</v>
       </c>
@@ -2759,7 +2880,7 @@
       </c>
       <c r="C111" s="4"/>
     </row>
-    <row r="112" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:3" ht="20.25" customHeight="1">
       <c r="A112" s="2" t="s">
         <v>6</v>
       </c>
@@ -2768,7 +2889,7 @@
       </c>
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:3" ht="20.25" customHeight="1">
       <c r="A113" s="2" t="s">
         <v>6</v>
       </c>
@@ -2777,7 +2898,7 @@
       </c>
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:3" ht="20.25" customHeight="1">
       <c r="A114" s="2" t="s">
         <v>6</v>
       </c>
@@ -2786,7 +2907,7 @@
       </c>
       <c r="C114" s="4"/>
     </row>
-    <row r="115" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:3" ht="20.25" customHeight="1">
       <c r="A115" s="2" t="s">
         <v>6</v>
       </c>
@@ -2795,7 +2916,7 @@
       </c>
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:3" ht="20.25" customHeight="1">
       <c r="A116" s="2" t="s">
         <v>6</v>
       </c>
@@ -2810,5 +2931,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added cmip6 mapings for cmip5 atmosphere scientific properties and exported as csv.
</commit_message>
<xml_diff>
--- a/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28480" yWindow="740" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="26500" yWindow="0" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="207">
   <si>
     <t>Atmosphere &gt; Convection Cloud Turbulence</t>
   </si>
@@ -439,6 +440,210 @@
   </si>
   <si>
     <t>cmip6.atmos.volcanos.volcanoes_treatment.volcanoes_implementation</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.boundary_layer_turbulence.closure_order</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.boundary_layer_turbulence.counter_gradient</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.boundary_layer_turbulence.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.boundary_layer_turbulence.scheme_type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.deep_convection.processes</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.deep_convection.scheme_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.deep_convection.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.deep_convection.scheme_type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.shallow_convection.scheme_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.shallow_convection.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.turbulence_convection.shallow_convection.scheme_type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.microphysics_precipitation.large_scale_precipitation.hydrometeors</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.microphysics_precipitation.large_scale_precipitation.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.microphysics_precipitation.cloud_microphysics.processes</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.microphysics_precipitation.cloud_microphysics.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.cosp_attributes.run_conviguration</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.cosp_attributes.number_of_columns</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.cosp_attributes.number_of_grid_points</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.cosp_attributes.number_of_levels</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.lidar_inputs.ice_types</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.lidar_inputs.overlap</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.radar_inputs.frequency</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.radar_inputs.type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.radar_inputs.effective_radius</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.radar_inputs.gas_absorption</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_scheme.cloud_overlap_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_scheme.uses_separate_treatment</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.top_boundary.top_heat</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.top_boundary.top_boundary_condition</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.top_boundary.top_wind</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.diffusion_horizontal.scheme_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.diffusion_horizontal.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.lateral_boundary.condition</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.prognostic_variables</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.timestepping_type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.advection_momentum.conservation_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.advection_momentum.conserved_quantities</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.advection_momentum.scheme_characteristics</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.advection_momentum.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.advection_momentum.scheme_staggering_type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.advection_tracers.conservation_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.advection_tracers.conserved_quantities</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.advection_tracers.scheme_characteristics</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.dynamical_core.advection_tracers.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.grid.discretisation.horizontal.scheme_type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.grid.discretisation.horizontal.horizontal_pole</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.grid.discretisation.horizontal.scheme_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.grid.discretisation.horizontal.scheme_order</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.background</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.sponge_layer</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.subgrid_scale_orography</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.non_orographic_gravity_waves.calculation_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.non_orographic_gravity_waves.dissipation_scheme</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.non_orographic_gravity_waves.propagation_scheme</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.non_orographic_gravity_waves.source_mechanisms</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.orographic_gravity_waves.calculation_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.orographic_gravity_waves.dissipation_scheme</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.orographic_gravity_waves.propagation_scheme</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.gravity_waves.orographic_gravity_waves.source_mechanisms</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.radiation.aerosols</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.radiation.greenhouse_gases</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.radiation.longwave_radiation.spectral_intervals</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.radiation.longwave_radiation.transport_calculation</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.radiation.longwave_radiation.spectral_integration</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.radiation.shortwave_radiation.spectral_intervals</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.radiation.shortwave_radiation.spectral_integration</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.key_properties.resolution.timestep_radiative_transfer</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.key_properties.resolution.timestep_dynamics</t>
   </si>
 </sst>
 </file>
@@ -590,8 +795,164 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -651,17 +1012,69 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1852,7 +2265,7 @@
   <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -2096,7 +2509,9 @@
       <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="20.25" customHeight="1">
       <c r="A24" s="2" t="s">
@@ -2105,7 +2520,9 @@
       <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="20.25" customHeight="1">
       <c r="A25" s="2" t="s">
@@ -2114,7 +2531,9 @@
       <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="7" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="20.25" customHeight="1">
       <c r="A26" s="2" t="s">
@@ -2123,7 +2542,9 @@
       <c r="B26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="7" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="20.25" customHeight="1">
       <c r="A27" s="2" t="s">
@@ -2132,7 +2553,6 @@
       <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" ht="20.25" customHeight="1">
       <c r="A28" s="2" t="s">
@@ -2141,7 +2561,9 @@
       <c r="B28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="7" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="20.25" customHeight="1">
       <c r="A29" s="2" t="s">
@@ -2150,7 +2572,9 @@
       <c r="B29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="7" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="20.25" customHeight="1">
       <c r="A30" s="2" t="s">
@@ -2159,7 +2583,9 @@
       <c r="B30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="20.25" customHeight="1">
       <c r="A31" s="2" t="s">
@@ -2168,7 +2594,9 @@
       <c r="B31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="7" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="20.25" customHeight="1">
       <c r="A32" s="2" t="s">
@@ -2177,7 +2605,9 @@
       <c r="B32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="20.25" customHeight="1">
       <c r="A33" s="2" t="s">
@@ -2186,7 +2616,9 @@
       <c r="B33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="20.25" customHeight="1">
       <c r="A34" s="2" t="s">
@@ -2195,7 +2627,9 @@
       <c r="B34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="7" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="20.25" customHeight="1">
       <c r="A35" s="2" t="s">
@@ -2204,7 +2638,9 @@
       <c r="B35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="7" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="20.25" customHeight="1">
       <c r="A36" s="2" t="s">
@@ -2231,7 +2667,9 @@
       <c r="B38" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="4"/>
+      <c r="C38" s="7" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="20.25" customHeight="1">
       <c r="A39" s="2" t="s">
@@ -2240,7 +2678,9 @@
       <c r="B39" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="4"/>
+      <c r="C39" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="20.25" customHeight="1">
       <c r="A40" s="2" t="s">
@@ -2249,7 +2689,9 @@
       <c r="B40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="4"/>
+      <c r="C40" s="7" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="20.25" customHeight="1">
       <c r="A41" s="2"/>
@@ -2263,7 +2705,9 @@
       <c r="B42" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="4"/>
+      <c r="C42" s="4" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="20.25" customHeight="1">
       <c r="A43" s="2" t="s">
@@ -2301,7 +2745,9 @@
       <c r="B46" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="4"/>
+      <c r="C46" s="4" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="20.25" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -2359,7 +2805,9 @@
       <c r="B52" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C52" s="4"/>
+      <c r="C52" s="4" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="53" spans="1:3" ht="20.25" customHeight="1">
       <c r="A53" s="2" t="s">
@@ -2368,7 +2816,9 @@
       <c r="B53" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C53" s="4"/>
+      <c r="C53" s="4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="54" spans="1:3" ht="20.25" customHeight="1">
       <c r="A54" s="2" t="s">
@@ -2377,7 +2827,9 @@
       <c r="B54" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="4"/>
+      <c r="C54" s="4" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="55" spans="1:3" ht="20.25" customHeight="1">
       <c r="A55" s="2" t="s">
@@ -2386,7 +2838,9 @@
       <c r="B55" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="4"/>
+      <c r="C55" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="56" spans="1:3" ht="20.25" customHeight="1">
       <c r="A56" s="2" t="s">
@@ -2417,7 +2871,9 @@
       <c r="B58" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C58" s="4"/>
+      <c r="C58" s="7" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="59" spans="1:3" ht="20.25" customHeight="1">
       <c r="A59" s="2" t="s">
@@ -2426,7 +2882,9 @@
       <c r="B59" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C59" s="4"/>
+      <c r="C59" s="7" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="60" spans="1:3" ht="20.25" customHeight="1">
       <c r="A60" s="2" t="s">
@@ -2435,7 +2893,9 @@
       <c r="B60" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C60" s="4"/>
+      <c r="C60" s="7" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="61" spans="1:3" ht="20.25" customHeight="1">
       <c r="A61" s="2" t="s">
@@ -2444,7 +2904,9 @@
       <c r="B61" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C61" s="4"/>
+      <c r="C61" s="7" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="62" spans="1:3" ht="20.25" customHeight="1">
       <c r="A62" s="2" t="s">
@@ -2453,7 +2915,9 @@
       <c r="B62" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C62" s="4"/>
+      <c r="C62" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="63" spans="1:3" ht="20.25" customHeight="1">
       <c r="A63" s="2" t="s">
@@ -2462,7 +2926,9 @@
       <c r="B63" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C63" s="4"/>
+      <c r="C63" s="7" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="64" spans="1:3" ht="20.25" customHeight="1">
       <c r="A64" s="2"/>
@@ -2476,7 +2942,9 @@
       <c r="B65" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C65" s="4"/>
+      <c r="C65" s="4" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="66" spans="1:3" ht="20.25" customHeight="1">
       <c r="A66" s="2" t="s">
@@ -2485,7 +2953,9 @@
       <c r="B66" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C66" s="4"/>
+      <c r="C66" s="4" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="67" spans="1:3" ht="20.25" customHeight="1">
       <c r="A67" s="2" t="s">
@@ -2494,7 +2964,9 @@
       <c r="B67" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C67" s="4"/>
+      <c r="C67" s="4" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="68" spans="1:3" ht="20.25" customHeight="1">
       <c r="A68" s="2" t="s">
@@ -2503,7 +2975,9 @@
       <c r="B68" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="4"/>
+      <c r="C68" s="4" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="69" spans="1:3" ht="20.25" customHeight="1">
       <c r="A69" s="2" t="s">
@@ -2512,7 +2986,9 @@
       <c r="B69" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C69" s="4"/>
+      <c r="C69" s="4" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="70" spans="1:3" ht="20.25" customHeight="1">
       <c r="A70" s="2" t="s">
@@ -2521,7 +2997,9 @@
       <c r="B70" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C70" s="4"/>
+      <c r="C70" s="4" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="71" spans="1:3" ht="20.25" customHeight="1">
       <c r="A71" s="2" t="s">
@@ -2530,7 +3008,9 @@
       <c r="B71" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C71" s="4"/>
+      <c r="C71" s="4" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="72" spans="1:3" ht="20.25" customHeight="1">
       <c r="A72" s="2" t="s">
@@ -2539,7 +3019,9 @@
       <c r="B72" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C72" s="4"/>
+      <c r="C72" s="7" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="73" spans="1:3" ht="20.25" customHeight="1">
       <c r="A73" s="2" t="s">
@@ -2548,7 +3030,9 @@
       <c r="B73" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C73" s="4"/>
+      <c r="C73" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="74" spans="1:3" ht="20.25" customHeight="1">
       <c r="A74" s="2" t="s">
@@ -2557,7 +3041,9 @@
       <c r="B74" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C74" s="4"/>
+      <c r="C74" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="75" spans="1:3" ht="20.25" customHeight="1">
       <c r="A75" s="2" t="s">
@@ -2566,7 +3052,9 @@
       <c r="B75" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C75" s="4"/>
+      <c r="C75" s="4" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="76" spans="1:3" ht="20.25" customHeight="1">
       <c r="A76" s="2" t="s">
@@ -2575,7 +3063,9 @@
       <c r="B76" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C76" s="4"/>
+      <c r="C76" s="4" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="77" spans="1:3" ht="20.25" customHeight="1">
       <c r="A77" s="2" t="s">
@@ -2584,7 +3074,9 @@
       <c r="B77" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C77" s="4"/>
+      <c r="C77" s="4" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="78" spans="1:3" ht="20.25" customHeight="1">
       <c r="A78" s="2"/>
@@ -2598,7 +3090,9 @@
       <c r="B79" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C79" s="4"/>
+      <c r="C79" s="4" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="80" spans="1:3" ht="20.25" customHeight="1">
       <c r="A80" s="2" t="s">
@@ -2607,7 +3101,9 @@
       <c r="B80" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C80" s="4"/>
+      <c r="C80" s="4" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="81" spans="1:3" ht="20.25" customHeight="1">
       <c r="A81" s="2" t="s">
@@ -2616,7 +3112,9 @@
       <c r="B81" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C81" s="4"/>
+      <c r="C81" s="4" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="82" spans="1:3" ht="20.25" customHeight="1">
       <c r="A82" s="2" t="s">
@@ -2625,7 +3123,9 @@
       <c r="B82" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C82" s="4"/>
+      <c r="C82" s="4" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="83" spans="1:3" ht="20.25" customHeight="1">
       <c r="A83" s="2" t="s">
@@ -2643,7 +3143,9 @@
       <c r="B84" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C84" s="4"/>
+      <c r="C84" s="4" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="85" spans="1:3" ht="20.25" customHeight="1">
       <c r="A85" s="2" t="s">
@@ -2652,7 +3154,9 @@
       <c r="B85" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C85" s="4"/>
+      <c r="C85" s="4" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="20.25" customHeight="1">
       <c r="A86" s="2" t="s">
@@ -2661,7 +3165,9 @@
       <c r="B86" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C86" s="4"/>
+      <c r="C86" s="4" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="87" spans="1:3" ht="20.25" customHeight="1">
       <c r="A87" s="2" t="s">
@@ -2670,7 +3176,9 @@
       <c r="B87" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C87" s="4"/>
+      <c r="C87" s="4" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="88" spans="1:3" ht="20.25" customHeight="1">
       <c r="A88" s="2" t="s">
@@ -2679,7 +3187,9 @@
       <c r="B88" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C88" s="4"/>
+      <c r="C88" s="4" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="89" spans="1:3" ht="20.25" customHeight="1">
       <c r="A89" s="2"/>
@@ -2693,7 +3203,9 @@
       <c r="B90" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C90" s="4"/>
+      <c r="C90" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="91" spans="1:3" ht="20.25" customHeight="1">
       <c r="A91" s="2" t="s">
@@ -2720,7 +3232,9 @@
       <c r="B93" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C93" s="4"/>
+      <c r="C93" s="4" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="94" spans="1:3" ht="20.25" customHeight="1">
       <c r="A94" s="2" t="s">
@@ -2729,7 +3243,9 @@
       <c r="B94" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C94" s="4"/>
+      <c r="C94" s="4" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="95" spans="1:3" ht="20.25" customHeight="1">
       <c r="A95" s="2" t="s">
@@ -2738,7 +3254,9 @@
       <c r="B95" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C95" s="4"/>
+      <c r="C95" s="4" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="96" spans="1:3" ht="20.25" customHeight="1">
       <c r="A96" s="2" t="s">
@@ -2747,7 +3265,9 @@
       <c r="B96" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C96" s="4"/>
+      <c r="C96" s="4" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="97" spans="1:3" ht="20.25" customHeight="1">
       <c r="A97" s="2" t="s">
@@ -2756,7 +3276,9 @@
       <c r="B97" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C97" s="4"/>
+      <c r="C97" s="4" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="98" spans="1:3" ht="20.25" customHeight="1">
       <c r="A98" s="2" t="s">
@@ -2774,7 +3296,9 @@
       <c r="B99" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C99" s="4"/>
+      <c r="C99" s="4" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="100" spans="1:3" ht="20.25" customHeight="1">
       <c r="A100" s="2" t="s">
@@ -2783,7 +3307,9 @@
       <c r="B100" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C100" s="4"/>
+      <c r="C100" s="4" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="101" spans="1:3" ht="20.25" customHeight="1">
       <c r="A101" s="2" t="s">
@@ -2792,7 +3318,9 @@
       <c r="B101" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C101" s="4"/>
+      <c r="C101" s="4" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="102" spans="1:3" ht="20.25" customHeight="1">
       <c r="A102" s="2" t="s">
@@ -2801,7 +3329,9 @@
       <c r="B102" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C102" s="4"/>
+      <c r="C102" s="4" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="103" spans="1:3" ht="20.25" customHeight="1">
       <c r="A103" s="2" t="s">
@@ -2810,7 +3340,9 @@
       <c r="B103" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C103" s="4"/>
+      <c r="C103" s="4" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="104" spans="1:3" ht="20.25" customHeight="1">
       <c r="A104" s="2"/>
@@ -2824,7 +3356,9 @@
       <c r="B105" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C105" s="4"/>
+      <c r="C105" s="4" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="106" spans="1:3" ht="20.25" customHeight="1">
       <c r="A106" s="2" t="s">
@@ -2851,7 +3385,9 @@
       <c r="B108" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C108" s="4"/>
+      <c r="C108" s="4" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="109" spans="1:3" ht="20.25" customHeight="1">
       <c r="A109" s="2" t="s">
@@ -2860,7 +3396,9 @@
       <c r="B109" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C109" s="4"/>
+      <c r="C109" s="4" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="110" spans="1:3" ht="20.25" customHeight="1">
       <c r="A110" s="2" t="s">
@@ -2869,7 +3407,9 @@
       <c r="B110" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C110" s="4"/>
+      <c r="C110" s="4" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="111" spans="1:3" ht="20.25" customHeight="1">
       <c r="A111" s="2" t="s">
@@ -2878,7 +3418,9 @@
       <c r="B111" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C111" s="4"/>
+      <c r="C111" s="4" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="112" spans="1:3" ht="20.25" customHeight="1">
       <c r="A112" s="2" t="s">
@@ -2896,7 +3438,9 @@
       <c r="B113" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C113" s="4"/>
+      <c r="C113" s="4" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="114" spans="1:3" ht="20.25" customHeight="1">
       <c r="A114" s="2" t="s">
@@ -2905,7 +3449,9 @@
       <c r="B114" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C114" s="4"/>
+      <c r="C114" s="4" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="115" spans="1:3" ht="20.25" customHeight="1">
       <c r="A115" s="2" t="s">
@@ -2923,7 +3469,9 @@
       <c r="B116" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C116" s="4"/>
+      <c r="C116" s="4" t="s">
+        <v>205</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -2937,4 +3485,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated mappings xlsx file
</commit_message>
<xml_diff>
--- a/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-atmos/mappings/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26500" yWindow="0" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -2268,7 +2272,7 @@
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="51.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2276,7 +2280,7 @@
     <col min="4" max="254" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="27" customHeight="1">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>127</v>
       </c>
@@ -2287,7 +2291,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+    <row r="2" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>126</v>
       </c>
@@ -2298,7 +2302,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+    <row r="3" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>126</v>
       </c>
@@ -2309,7 +2313,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>126</v>
       </c>
@@ -2320,7 +2324,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>126</v>
       </c>
@@ -2331,7 +2335,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1">
+    <row r="6" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>126</v>
       </c>
@@ -2342,7 +2346,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1">
+    <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>126</v>
       </c>
@@ -2353,7 +2357,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1">
+    <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>126</v>
       </c>
@@ -2364,7 +2368,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1">
+    <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>126</v>
       </c>
@@ -2373,7 +2377,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1">
+    <row r="10" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>126</v>
       </c>
@@ -2382,7 +2386,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1">
+    <row r="11" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>126</v>
       </c>
@@ -2393,7 +2397,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1">
+    <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>126</v>
       </c>
@@ -2404,7 +2408,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1">
+    <row r="13" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>126</v>
       </c>
@@ -2415,7 +2419,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1">
+    <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>126</v>
       </c>
@@ -2424,7 +2428,7 @@
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1">
+    <row r="15" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>126</v>
       </c>
@@ -2435,7 +2439,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1">
+    <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>126</v>
       </c>
@@ -2446,7 +2450,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1">
+    <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>126</v>
       </c>
@@ -2457,7 +2461,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1">
+    <row r="18" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>126</v>
       </c>
@@ -2468,7 +2472,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1">
+    <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>126</v>
       </c>
@@ -2479,7 +2483,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1">
+    <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>126</v>
       </c>
@@ -2488,7 +2492,7 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1">
+    <row r="21" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>126</v>
       </c>
@@ -2497,12 +2501,12 @@
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1">
+    <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="20.25" customHeight="1">
+    <row r="23" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2517,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="20.25" customHeight="1">
+    <row r="24" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -2524,7 +2528,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="20.25" customHeight="1">
+    <row r="25" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -2535,7 +2539,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="20.25" customHeight="1">
+    <row r="26" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -2546,7 +2550,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="20.25" customHeight="1">
+    <row r="27" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="20.25" customHeight="1">
+    <row r="28" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -2565,7 +2569,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="20.25" customHeight="1">
+    <row r="29" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -2576,7 +2580,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="20.25" customHeight="1">
+    <row r="30" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -2587,7 +2591,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="20.25" customHeight="1">
+    <row r="31" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="20.25" customHeight="1">
+    <row r="32" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2609,7 +2613,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="20.25" customHeight="1">
+    <row r="33" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2620,7 +2624,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="20.25" customHeight="1">
+    <row r="34" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -2631,7 +2635,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="20.25" customHeight="1">
+    <row r="35" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -2642,7 +2646,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="20.25" customHeight="1">
+    <row r="36" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -2651,7 +2655,7 @@
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" ht="20.25" customHeight="1">
+    <row r="37" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -2660,7 +2664,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" ht="20.25" customHeight="1">
+    <row r="38" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +2675,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="20.25" customHeight="1">
+    <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
@@ -2682,7 +2686,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="20.25" customHeight="1">
+    <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
@@ -2693,12 +2697,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="20.25" customHeight="1">
+    <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="20.25" customHeight="1">
+    <row r="42" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
@@ -2709,7 +2713,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="20.25" customHeight="1">
+    <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>1</v>
       </c>
@@ -2718,7 +2722,7 @@
       </c>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="20.25" customHeight="1">
+    <row r="44" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>1</v>
       </c>
@@ -2729,7 +2733,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="20.25" customHeight="1">
+    <row r="45" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
@@ -2738,7 +2742,7 @@
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" ht="20.25" customHeight="1">
+    <row r="46" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>1</v>
       </c>
@@ -2749,7 +2753,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="20.25" customHeight="1">
+    <row r="47" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>1</v>
       </c>
@@ -2760,7 +2764,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="20.25" customHeight="1">
+    <row r="48" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
@@ -2771,7 +2775,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="20.25" customHeight="1">
+    <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>1</v>
       </c>
@@ -2782,7 +2786,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="20.25" customHeight="1">
+    <row r="50" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
@@ -2793,12 +2797,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="20.25" customHeight="1">
+    <row r="51" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" ht="20.25" customHeight="1">
+    <row r="52" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
@@ -2809,7 +2813,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="20.25" customHeight="1">
+    <row r="53" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
@@ -2820,7 +2824,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="20.25" customHeight="1">
+    <row r="54" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>2</v>
       </c>
@@ -2831,7 +2835,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="20.25" customHeight="1">
+    <row r="55" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
@@ -2842,7 +2846,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="20.25" customHeight="1">
+    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2853,7 +2857,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="20.25" customHeight="1">
+    <row r="57" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
@@ -2864,7 +2868,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="20.25" customHeight="1">
+    <row r="58" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
@@ -2875,7 +2879,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="20.25" customHeight="1">
+    <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
@@ -2886,7 +2890,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="20.25" customHeight="1">
+    <row r="60" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
@@ -2897,7 +2901,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="20.25" customHeight="1">
+    <row r="61" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
@@ -2908,7 +2912,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="20.25" customHeight="1">
+    <row r="62" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -2919,7 +2923,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="20.25" customHeight="1">
+    <row r="63" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -2930,12 +2934,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="20.25" customHeight="1">
+    <row r="64" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="1:3" ht="20.25" customHeight="1">
+    <row r="65" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="2" t="s">
         <v>3</v>
       </c>
@@ -2946,7 +2950,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="20.25" customHeight="1">
+    <row r="66" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="2" t="s">
         <v>3</v>
       </c>
@@ -2957,7 +2961,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="20.25" customHeight="1">
+    <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="2" t="s">
         <v>3</v>
       </c>
@@ -2968,7 +2972,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="20.25" customHeight="1">
+    <row r="68" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="2" t="s">
         <v>3</v>
       </c>
@@ -2979,7 +2983,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="20.25" customHeight="1">
+    <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="2" t="s">
         <v>3</v>
       </c>
@@ -2990,7 +2994,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="20.25" customHeight="1">
+    <row r="70" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -3001,7 +3005,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="20.25" customHeight="1">
+    <row r="71" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -3012,7 +3016,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="20.25" customHeight="1">
+    <row r="72" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="2" t="s">
         <v>3</v>
       </c>
@@ -3023,7 +3027,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="20.25" customHeight="1">
+    <row r="73" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="2" t="s">
         <v>3</v>
       </c>
@@ -3034,7 +3038,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="20.25" customHeight="1">
+    <row r="74" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="2" t="s">
         <v>3</v>
       </c>
@@ -3045,7 +3049,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="20.25" customHeight="1">
+    <row r="75" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="2" t="s">
         <v>3</v>
       </c>
@@ -3056,7 +3060,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="20.25" customHeight="1">
+    <row r="76" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -3067,7 +3071,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="20.25" customHeight="1">
+    <row r="77" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="2" t="s">
         <v>3</v>
       </c>
@@ -3078,12 +3082,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="20.25" customHeight="1">
+    <row r="78" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="1:3" ht="20.25" customHeight="1">
+    <row r="79" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="2" t="s">
         <v>4</v>
       </c>
@@ -3094,7 +3098,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="20.25" customHeight="1">
+    <row r="80" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="2" t="s">
         <v>4</v>
       </c>
@@ -3105,7 +3109,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="20.25" customHeight="1">
+    <row r="81" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="2" t="s">
         <v>4</v>
       </c>
@@ -3116,7 +3120,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="20.25" customHeight="1">
+    <row r="82" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="2" t="s">
         <v>4</v>
       </c>
@@ -3127,7 +3131,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="20.25" customHeight="1">
+    <row r="83" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="2" t="s">
         <v>4</v>
       </c>
@@ -3136,7 +3140,7 @@
       </c>
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="1:3" ht="20.25" customHeight="1">
+    <row r="84" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="2" t="s">
         <v>4</v>
       </c>
@@ -3147,7 +3151,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="20.25" customHeight="1">
+    <row r="85" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
         <v>4</v>
       </c>
@@ -3158,7 +3162,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="20.25" customHeight="1">
+    <row r="86" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="2" t="s">
         <v>4</v>
       </c>
@@ -3169,7 +3173,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="20.25" customHeight="1">
+    <row r="87" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="2" t="s">
         <v>4</v>
       </c>
@@ -3180,7 +3184,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="20.25" customHeight="1">
+    <row r="88" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="2" t="s">
         <v>4</v>
       </c>
@@ -3191,12 +3195,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="20.25" customHeight="1">
+    <row r="89" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="1:3" ht="20.25" customHeight="1">
+    <row r="90" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="2" t="s">
         <v>5</v>
       </c>
@@ -3207,7 +3211,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="20.25" customHeight="1">
+    <row r="91" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="2" t="s">
         <v>5</v>
       </c>
@@ -3216,7 +3220,7 @@
       </c>
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="1:3" ht="20.25" customHeight="1">
+    <row r="92" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="2" t="s">
         <v>5</v>
       </c>
@@ -3225,7 +3229,7 @@
       </c>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="1:3" ht="20.25" customHeight="1">
+    <row r="93" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="2" t="s">
         <v>5</v>
       </c>
@@ -3236,7 +3240,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="20.25" customHeight="1">
+    <row r="94" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="2" t="s">
         <v>5</v>
       </c>
@@ -3247,7 +3251,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="20.25" customHeight="1">
+    <row r="95" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="2" t="s">
         <v>5</v>
       </c>
@@ -3258,7 +3262,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="20.25" customHeight="1">
+    <row r="96" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="2" t="s">
         <v>5</v>
       </c>
@@ -3269,7 +3273,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="20.25" customHeight="1">
+    <row r="97" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="2" t="s">
         <v>5</v>
       </c>
@@ -3280,7 +3284,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="20.25" customHeight="1">
+    <row r="98" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="2" t="s">
         <v>5</v>
       </c>
@@ -3289,7 +3293,7 @@
       </c>
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="1:3" ht="20.25" customHeight="1">
+    <row r="99" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="2" t="s">
         <v>5</v>
       </c>
@@ -3300,7 +3304,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="20.25" customHeight="1">
+    <row r="100" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="2" t="s">
         <v>5</v>
       </c>
@@ -3311,7 +3315,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="20.25" customHeight="1">
+    <row r="101" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
         <v>5</v>
       </c>
@@ -3322,7 +3326,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="20.25" customHeight="1">
+    <row r="102" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="2" t="s">
         <v>5</v>
       </c>
@@ -3333,7 +3337,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="20.25" customHeight="1">
+    <row r="103" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="2" t="s">
         <v>5</v>
       </c>
@@ -3344,12 +3348,12 @@
         <v>189</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="20.25" customHeight="1">
+    <row r="104" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="1:3" ht="20.25" customHeight="1">
+    <row r="105" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="2" t="s">
         <v>6</v>
       </c>
@@ -3360,7 +3364,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="20.25" customHeight="1">
+    <row r="106" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="2" t="s">
         <v>6</v>
       </c>
@@ -3369,7 +3373,7 @@
       </c>
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="1:3" ht="20.25" customHeight="1">
+    <row r="107" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="2" t="s">
         <v>6</v>
       </c>
@@ -3378,7 +3382,7 @@
       </c>
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="1:3" ht="20.25" customHeight="1">
+    <row r="108" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="2" t="s">
         <v>6</v>
       </c>
@@ -3389,7 +3393,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="20.25" customHeight="1">
+    <row r="109" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
         <v>6</v>
       </c>
@@ -3400,7 +3404,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="20.25" customHeight="1">
+    <row r="110" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="2" t="s">
         <v>6</v>
       </c>
@@ -3411,7 +3415,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="20.25" customHeight="1">
+    <row r="111" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="2" t="s">
         <v>6</v>
       </c>
@@ -3422,7 +3426,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="20.25" customHeight="1">
+    <row r="112" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="2" t="s">
         <v>6</v>
       </c>
@@ -3431,7 +3435,7 @@
       </c>
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="1:3" ht="20.25" customHeight="1">
+    <row r="113" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="2" t="s">
         <v>6</v>
       </c>
@@ -3442,7 +3446,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="20.25" customHeight="1">
+    <row r="114" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="2" t="s">
         <v>6</v>
       </c>
@@ -3453,7 +3457,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="20.25" customHeight="1">
+    <row r="115" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="2" t="s">
         <v>6</v>
       </c>
@@ -3462,7 +3466,7 @@
       </c>
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="1:3" ht="20.25" customHeight="1">
+    <row r="116" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="2" t="s">
         <v>6</v>
       </c>
@@ -3479,27 +3483,5 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tooling comments improved.  Artefacst regenerated.  Mapping typos fixed.
</commit_message>
<xml_diff>
--- a/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -419,9 +419,6 @@
     <t>CMIP6 Specialization ID</t>
   </si>
   <si>
-    <t>cmip6.atmos.solar/insolation_ozone.solar_ozone_impact</t>
-  </si>
-  <si>
     <t>cmip6.atmos.solar.orbital_parameters.computation_method</t>
   </si>
   <si>
@@ -491,9 +488,6 @@
     <t>cmip6.atmos.microphysics_precipitation.cloud_microphysics.scheme_name</t>
   </si>
   <si>
-    <t>cmip6.atmos.cloud_simulator.cosp_attributes.run_conviguration</t>
-  </si>
-  <si>
     <t>cmip6.atmos.cloud_simulator.cosp_attributes.number_of_columns</t>
   </si>
   <si>
@@ -648,6 +642,12 @@
   </si>
   <si>
     <t>cmip6.atmos.key_properties.resolution.timestep_dynamics</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.insolation_ozone.solar_ozone_impact</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_simulator.cosp_attributes.run_configuration</t>
   </si>
 </sst>
 </file>
@@ -2268,8 +2268,8 @@
   </sheetPr>
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2342,8 +2342,8 @@
       <c r="B6" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>130</v>
+      <c r="C6" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2354,7 +2354,7 @@
         <v>111</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2365,7 +2365,7 @@
         <v>112</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2394,7 +2394,7 @@
         <v>115</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2405,7 +2405,7 @@
         <v>116</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2416,7 +2416,7 @@
         <v>117</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2436,7 +2436,7 @@
         <v>119</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2447,7 +2447,7 @@
         <v>120</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2458,7 +2458,7 @@
         <v>121</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2469,7 +2469,7 @@
         <v>122</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2480,7 +2480,7 @@
         <v>123</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2514,7 +2514,7 @@
         <v>7</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2525,7 +2525,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2536,7 +2536,7 @@
         <v>9</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2547,7 +2547,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2566,7 +2566,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2577,7 +2577,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2588,7 +2588,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2599,7 +2599,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2610,7 +2610,7 @@
         <v>16</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2621,7 +2621,7 @@
         <v>17</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2632,7 +2632,7 @@
         <v>18</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2643,7 +2643,7 @@
         <v>19</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2672,7 +2672,7 @@
         <v>22</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2683,7 +2683,7 @@
         <v>23</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2694,7 +2694,7 @@
         <v>24</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2710,7 +2710,7 @@
         <v>25</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2750,7 +2750,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2809,8 +2809,8 @@
       <c r="B52" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>154</v>
+      <c r="C52" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2821,7 +2821,7 @@
         <v>35</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2832,7 +2832,7 @@
         <v>36</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2843,7 +2843,7 @@
         <v>37</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2876,7 +2876,7 @@
         <v>40</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2887,7 +2887,7 @@
         <v>41</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2898,7 +2898,7 @@
         <v>42</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2909,7 +2909,7 @@
         <v>43</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2920,7 +2920,7 @@
         <v>44</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2931,7 +2931,7 @@
         <v>45</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2947,7 +2947,7 @@
         <v>46</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2958,7 +2958,7 @@
         <v>47</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2969,7 +2969,7 @@
         <v>48</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2980,7 +2980,7 @@
         <v>49</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2991,7 +2991,7 @@
         <v>50</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3002,7 +3002,7 @@
         <v>51</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3013,7 +3013,7 @@
         <v>52</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3024,7 +3024,7 @@
         <v>53</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3035,7 +3035,7 @@
         <v>54</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3046,7 +3046,7 @@
         <v>55</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3057,7 +3057,7 @@
         <v>56</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3068,7 +3068,7 @@
         <v>57</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3079,7 +3079,7 @@
         <v>58</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3095,7 +3095,7 @@
         <v>59</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3106,7 +3106,7 @@
         <v>60</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3117,7 +3117,7 @@
         <v>61</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3128,7 +3128,7 @@
         <v>62</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3148,7 +3148,7 @@
         <v>64</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3159,7 +3159,7 @@
         <v>65</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3170,7 +3170,7 @@
         <v>66</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3181,7 +3181,7 @@
         <v>67</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3192,7 +3192,7 @@
         <v>68</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3208,7 +3208,7 @@
         <v>69</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3237,7 +3237,7 @@
         <v>72</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3248,7 +3248,7 @@
         <v>73</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3259,7 +3259,7 @@
         <v>74</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3270,7 +3270,7 @@
         <v>75</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3281,7 +3281,7 @@
         <v>76</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3301,7 +3301,7 @@
         <v>78</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3312,7 +3312,7 @@
         <v>79</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3323,7 +3323,7 @@
         <v>80</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3334,7 +3334,7 @@
         <v>81</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3345,7 +3345,7 @@
         <v>82</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3361,7 +3361,7 @@
         <v>83</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3390,7 +3390,7 @@
         <v>86</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3401,7 +3401,7 @@
         <v>87</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3412,7 +3412,7 @@
         <v>88</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3423,7 +3423,7 @@
         <v>89</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3443,7 +3443,7 @@
         <v>91</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3454,7 +3454,7 @@
         <v>92</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3474,7 +3474,7 @@
         <v>94</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CMIP5 to CMIP6 mappings.  Minor corrections to dynamical_core and observation_simulation e.g. spelling, indentation, hyphenation.
</commit_message>
<xml_diff>
--- a/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-atmos/mappings/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="208">
   <si>
     <t>Atmosphere &gt; Convection Cloud Turbulence</t>
   </si>
@@ -329,12 +324,6 @@
     <t>cmip6.atmos.cloud_scheme.processes</t>
   </si>
   <si>
-    <t>cmip6.atmos.cloud_simulator.isscp_attributes.top_height</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.isscp_attributes.top_height_direction</t>
-  </si>
-  <si>
     <t>Basic Approximations</t>
   </si>
   <si>
@@ -482,42 +471,6 @@
     <t>cmip6.atmos.microphysics_precipitation.large_scale_precipitation.scheme_name</t>
   </si>
   <si>
-    <t>cmip6.atmos.microphysics_precipitation.cloud_microphysics.processes</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.microphysics_precipitation.cloud_microphysics.scheme_name</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.cosp_attributes.number_of_columns</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.cosp_attributes.number_of_grid_points</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.cosp_attributes.number_of_levels</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.lidar_inputs.ice_types</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.lidar_inputs.overlap</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.radar_inputs.frequency</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.radar_inputs.type</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.radar_inputs.effective_radius</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_simulator.radar_inputs.gas_absorption</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.cloud_scheme.cloud_overlap_method</t>
-  </si>
-  <si>
     <t>cmip6.atmos.cloud_scheme.uses_separate_treatment</t>
   </si>
   <si>
@@ -620,9 +573,6 @@
     <t>cmip6.atmos.radiation.aerosols</t>
   </si>
   <si>
-    <t>cmip6.atmos.radiation.greenhouse_gases</t>
-  </si>
-  <si>
     <t>cmip6.atmos.radiation.longwave_radiation.spectral_intervals</t>
   </si>
   <si>
@@ -647,7 +597,55 @@
     <t>cmip6.atmos.solar.insolation_ozone.solar_ozone_impact</t>
   </si>
   <si>
-    <t>cmip6.atmos.cloud_simulator.cosp_attributes.run_configuration</t>
+    <t>cmip6.atmos.microphysics_precipitation.large_scale_cloud_microphysics.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.microphysics_precipitation.large_scale_cloud_microphysics.processes</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_scheme.optical_cloud_properties.cloud_overlap_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_scheme.prognostic_scheme</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.cosp_attributes.run_configuration</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.cosp_attributes.number_of_grid_points</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.cosp_attributes.number_of_levels</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.isscp_attributes.top_height_direction</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.lidar_inputs.ice_types</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.lidar_inputs.overlap</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.radar_inputs.frequency</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.radar_inputs.type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.radar_inputs.effective_radius</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.radar_inputs.gas_absorption</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.isscp_attributes.top_height_estimation_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.observation_simulation.cosp_attributes.number_of_sub_columns</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.radiation.lw_ghg.greenhouse.gas.complexity</t>
   </si>
 </sst>
 </file>
@@ -799,8 +797,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1016,7 +1050,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1048,6 +1082,12 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1079,6 +1119,12 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2268,11 +2314,11 @@
   </sheetPr>
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="51.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2280,233 +2326,233 @@
     <col min="4" max="254" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="27" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="20" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="5" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="20" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="20" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" ht="20" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="4" t="s">
+    <row r="12" spans="1:3" ht="20" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="20" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="4" t="s">
+    <row r="14" spans="1:3" ht="20" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" ht="20" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" s="4" t="s">
+    <row r="16" spans="1:3" ht="20" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="20" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="3" t="s">
+    <row r="18" spans="1:3" ht="20" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="20" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="3" t="s">
+    <row r="20" spans="1:3" ht="20" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" ht="20" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="20" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="20.25" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -2514,10 +2560,10 @@
         <v>7</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="20.25" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -2525,10 +2571,10 @@
         <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="20.25" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -2536,10 +2582,10 @@
         <v>9</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="20.25" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -2547,10 +2593,10 @@
         <v>10</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="20.25" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -2558,7 +2604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="20.25" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -2566,10 +2612,10 @@
         <v>12</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="20.25" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -2577,10 +2623,10 @@
         <v>13</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="20.25" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -2588,10 +2634,10 @@
         <v>14</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="20.25" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2599,10 +2645,10 @@
         <v>15</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="20.25" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2610,10 +2656,10 @@
         <v>16</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="20.25" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2621,32 +2667,32 @@
         <v>17</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="20.25" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C34" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="20.25" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C35" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="20.25" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -2655,7 +2701,7 @@
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="20.25" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -2664,7 +2710,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="20.25" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -2672,10 +2718,10 @@
         <v>22</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20.25" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
@@ -2683,10 +2729,10 @@
         <v>23</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20.25" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
@@ -2694,15 +2740,15 @@
         <v>24</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="20.25" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="20.25" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
@@ -2710,10 +2756,10 @@
         <v>25</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="20.25" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>1</v>
       </c>
@@ -2722,7 +2768,7 @@
       </c>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" ht="20.25" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>1</v>
       </c>
@@ -2733,16 +2779,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" ht="20.25" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C45" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="20.25" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>1</v>
       </c>
@@ -2750,10 +2798,10 @@
         <v>29</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="20.25" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>1</v>
       </c>
@@ -2764,7 +2812,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="20.25" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
@@ -2775,7 +2823,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="20.25" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>1</v>
       </c>
@@ -2786,7 +2834,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="20.25" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
@@ -2797,12 +2845,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="20.25" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="20.25" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
@@ -2810,10 +2858,10 @@
         <v>34</v>
       </c>
       <c r="C52" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="20.25" customHeight="1">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
@@ -2821,10 +2869,10 @@
         <v>35</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="20.25" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>2</v>
       </c>
@@ -2832,10 +2880,10 @@
         <v>36</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="20.25" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
@@ -2843,10 +2891,10 @@
         <v>37</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="20.25" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2854,10 +2902,10 @@
         <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="20.25" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
@@ -2865,10 +2913,10 @@
         <v>39</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="20.25" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
@@ -2876,10 +2924,10 @@
         <v>40</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="20.25" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
@@ -2887,10 +2935,10 @@
         <v>41</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="20.25" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
@@ -2898,10 +2946,10 @@
         <v>42</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="20.25" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
@@ -2909,10 +2957,10 @@
         <v>43</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="20.25" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -2920,10 +2968,10 @@
         <v>44</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="20.25" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -2931,15 +2979,15 @@
         <v>45</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="20.25" customHeight="1">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" ht="20.25" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>3</v>
       </c>
@@ -2947,10 +2995,10 @@
         <v>46</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="20.25" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>3</v>
       </c>
@@ -2958,10 +3006,10 @@
         <v>47</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="20.25" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>3</v>
       </c>
@@ -2969,10 +3017,10 @@
         <v>48</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="20.25" customHeight="1">
       <c r="A68" s="2" t="s">
         <v>3</v>
       </c>
@@ -2980,10 +3028,10 @@
         <v>49</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="20.25" customHeight="1">
       <c r="A69" s="2" t="s">
         <v>3</v>
       </c>
@@ -2991,10 +3039,10 @@
         <v>50</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="20.25" customHeight="1">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -3002,10 +3050,10 @@
         <v>51</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="20.25" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -3013,10 +3061,10 @@
         <v>52</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="20.25" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>3</v>
       </c>
@@ -3024,10 +3072,10 @@
         <v>53</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="20.25" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>3</v>
       </c>
@@ -3035,10 +3083,10 @@
         <v>54</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="20.25" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>3</v>
       </c>
@@ -3046,10 +3094,10 @@
         <v>55</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="20.25" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>3</v>
       </c>
@@ -3057,10 +3105,10 @@
         <v>56</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="20.25" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -3068,10 +3116,10 @@
         <v>57</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="20.25" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>3</v>
       </c>
@@ -3079,15 +3127,15 @@
         <v>58</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="20.25" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:3" ht="20.25" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>4</v>
       </c>
@@ -3095,10 +3143,10 @@
         <v>59</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="20.25" customHeight="1">
       <c r="A80" s="2" t="s">
         <v>4</v>
       </c>
@@ -3106,10 +3154,10 @@
         <v>60</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="20.25" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>4</v>
       </c>
@@ -3117,10 +3165,10 @@
         <v>61</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="20.25" customHeight="1">
       <c r="A82" s="2" t="s">
         <v>4</v>
       </c>
@@ -3128,10 +3176,10 @@
         <v>62</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="20.25" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>4</v>
       </c>
@@ -3140,7 +3188,7 @@
       </c>
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:3" ht="20.25" customHeight="1">
       <c r="A84" s="2" t="s">
         <v>4</v>
       </c>
@@ -3148,10 +3196,10 @@
         <v>64</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="20.25" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>4</v>
       </c>
@@ -3159,10 +3207,10 @@
         <v>65</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="20.25" customHeight="1">
       <c r="A86" s="2" t="s">
         <v>4</v>
       </c>
@@ -3170,10 +3218,10 @@
         <v>66</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="20.25" customHeight="1">
       <c r="A87" s="2" t="s">
         <v>4</v>
       </c>
@@ -3181,10 +3229,10 @@
         <v>67</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="20.25" customHeight="1">
       <c r="A88" s="2" t="s">
         <v>4</v>
       </c>
@@ -3192,15 +3240,15 @@
         <v>68</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="20.25" customHeight="1">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:3" ht="20.25" customHeight="1">
       <c r="A90" s="2" t="s">
         <v>5</v>
       </c>
@@ -3208,10 +3256,10 @@
         <v>69</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="20.25" customHeight="1">
       <c r="A91" s="2" t="s">
         <v>5</v>
       </c>
@@ -3220,7 +3268,7 @@
       </c>
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:3" ht="20.25" customHeight="1">
       <c r="A92" s="2" t="s">
         <v>5</v>
       </c>
@@ -3229,7 +3277,7 @@
       </c>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:3" ht="20.25" customHeight="1">
       <c r="A93" s="2" t="s">
         <v>5</v>
       </c>
@@ -3237,10 +3285,10 @@
         <v>72</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="20.25" customHeight="1">
       <c r="A94" s="2" t="s">
         <v>5</v>
       </c>
@@ -3248,10 +3296,10 @@
         <v>73</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="20.25" customHeight="1">
       <c r="A95" s="2" t="s">
         <v>5</v>
       </c>
@@ -3259,10 +3307,10 @@
         <v>74</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="20.25" customHeight="1">
       <c r="A96" s="2" t="s">
         <v>5</v>
       </c>
@@ -3270,10 +3318,10 @@
         <v>75</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="20.25" customHeight="1">
       <c r="A97" s="2" t="s">
         <v>5</v>
       </c>
@@ -3281,10 +3329,10 @@
         <v>76</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="20.25" customHeight="1">
       <c r="A98" s="2" t="s">
         <v>5</v>
       </c>
@@ -3293,7 +3341,7 @@
       </c>
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:3" ht="20.25" customHeight="1">
       <c r="A99" s="2" t="s">
         <v>5</v>
       </c>
@@ -3301,10 +3349,10 @@
         <v>78</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="20.25" customHeight="1">
       <c r="A100" s="2" t="s">
         <v>5</v>
       </c>
@@ -3312,10 +3360,10 @@
         <v>79</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="20.25" customHeight="1">
       <c r="A101" s="2" t="s">
         <v>5</v>
       </c>
@@ -3323,10 +3371,10 @@
         <v>80</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="20.25" customHeight="1">
       <c r="A102" s="2" t="s">
         <v>5</v>
       </c>
@@ -3334,10 +3382,10 @@
         <v>81</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="20.25" customHeight="1">
       <c r="A103" s="2" t="s">
         <v>5</v>
       </c>
@@ -3345,15 +3393,15 @@
         <v>82</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="20.25" customHeight="1">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:3" ht="20.25" customHeight="1">
       <c r="A105" s="2" t="s">
         <v>6</v>
       </c>
@@ -3361,10 +3409,10 @@
         <v>83</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="20.25" customHeight="1">
       <c r="A106" s="2" t="s">
         <v>6</v>
       </c>
@@ -3373,7 +3421,7 @@
       </c>
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:3" ht="20.25" customHeight="1">
       <c r="A107" s="2" t="s">
         <v>6</v>
       </c>
@@ -3382,7 +3430,7 @@
       </c>
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:3" ht="20.25" customHeight="1">
       <c r="A108" s="2" t="s">
         <v>6</v>
       </c>
@@ -3390,10 +3438,10 @@
         <v>86</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="20.25" customHeight="1">
       <c r="A109" s="2" t="s">
         <v>6</v>
       </c>
@@ -3401,10 +3449,10 @@
         <v>87</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="20.25" customHeight="1">
       <c r="A110" s="2" t="s">
         <v>6</v>
       </c>
@@ -3412,10 +3460,10 @@
         <v>88</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="20.25" customHeight="1">
       <c r="A111" s="2" t="s">
         <v>6</v>
       </c>
@@ -3423,10 +3471,10 @@
         <v>89</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="20.25" customHeight="1">
       <c r="A112" s="2" t="s">
         <v>6</v>
       </c>
@@ -3435,7 +3483,7 @@
       </c>
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:3" ht="20.25" customHeight="1">
       <c r="A113" s="2" t="s">
         <v>6</v>
       </c>
@@ -3443,10 +3491,10 @@
         <v>91</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="20.25" customHeight="1">
       <c r="A114" s="2" t="s">
         <v>6</v>
       </c>
@@ -3454,10 +3502,10 @@
         <v>92</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="20.25" customHeight="1">
       <c r="A115" s="2" t="s">
         <v>6</v>
       </c>
@@ -3466,7 +3514,7 @@
       </c>
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:3" ht="20.25" customHeight="1">
       <c r="A116" s="2" t="s">
         <v>6</v>
       </c>
@@ -3474,7 +3522,7 @@
         <v>94</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3483,5 +3531,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected mapping for atmosphere radiation GHG-types
</commit_message>
<xml_diff>
--- a/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/atmos-cmip5-to-cmip6-mappings.xlsx
@@ -645,7 +645,7 @@
     <t>cmip6.atmos.observation_simulation.cosp_attributes.number_of_sub_columns</t>
   </si>
   <si>
-    <t>cmip6.atmos.radiation.lw_ghg.greenhouse.gas.complexity</t>
+    <t>cmip6.atmos.radiation.longwave_GHG.greenhouse_gas_complexity</t>
   </si>
 </sst>
 </file>
@@ -2314,8 +2314,8 @@
   </sheetPr>
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>